<commit_message>
correjí errores de filtro
</commit_message>
<xml_diff>
--- a/excel/Estructura Nuevo Calendario final.xlsx
+++ b/excel/Estructura Nuevo Calendario final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{16003727-C6EF-4AB6-81B8-B898A4348C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A835FF21-FEC9-4453-B2E7-4869EE4D302F}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades" sheetId="1" r:id="rId1"/>
@@ -2149,6 +2149,20 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2172,20 +2186,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2250,7 +2250,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23C9AAE3-6A05-441D-9C0C-A139DBB9725F}" name="Table2" displayName="Table2" ref="H1:H1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23C9AAE3-6A05-441D-9C0C-A139DBB9725F}" name="Table2" displayName="Table2" ref="H1:H1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="H1:H1048576" xr:uid="{472508D3-5691-45D4-9E62-6DF8E7CBD8CD}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{FB77FFB4-73E4-44F2-9724-F1C1943BF17F}" name="programa"/>
@@ -2558,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F127" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H268"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>